<commit_message>
added log message and an if condition in test cases
</commit_message>
<xml_diff>
--- a/yourLogoDatas.xlsx
+++ b/yourLogoDatas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kali_\eclipse-Newworkspace\yourLogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77315A2E-3325-4E31-AD9F-AD73C06264ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15139AAE-D5B4-4B8F-BAE2-295D87BD3CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3551AA9-00BD-4D11-8AEC-E56200EE14DA}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changes in data values
</commit_message>
<xml_diff>
--- a/yourLogoDatas.xlsx
+++ b/yourLogoDatas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kali_\eclipse-Newworkspace\yourLogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15139AAE-D5B4-4B8F-BAE2-295D87BD3CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259DC38-08FD-4DF2-8CA8-34698698C9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3551AA9-00BD-4D11-8AEC-E56200EE14DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3551AA9-00BD-4D11-8AEC-E56200EE14DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Email ID</t>
-  </si>
-  <si>
     <t>cde@gmail.com</t>
   </si>
   <si>
@@ -104,18 +101,6 @@
     <t>MR</t>
   </si>
   <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Tyson</t>
-  </si>
-  <si>
-    <t>fgh@gmail.com</t>
-  </si>
-  <si>
-    <t>miket123</t>
-  </si>
-  <si>
     <t>March</t>
   </si>
   <si>
@@ -128,10 +113,19 @@
     <t>California</t>
   </si>
   <si>
-    <t>alias address of mike tyson</t>
-  </si>
-  <si>
     <t>cde123@gmail.com</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Skotia</t>
+  </si>
+  <si>
+    <t>novas123</t>
+  </si>
+  <si>
+    <t>alias address of nova skotia</t>
   </si>
 </sst>
 </file>
@@ -521,63 +515,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1AEBCE-B3D5-485A-A0C1-864F01E96AA8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8698C334-9E73-465C-B198-F132BC9B7278}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{FDCA88AA-B917-4CA9-BC90-68F2CC0E54ED}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{5DCADE5D-A32B-40D3-9746-110C3D720A48}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FDCA88AA-B917-4CA9-BC90-68F2CC0E54ED}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5DCADE5D-A32B-40D3-9746-110C3D720A48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -585,15 +569,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56106EF-C9CF-4A63-9C69-6091709BFB07}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="10" max="10" width="11.77734375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
@@ -602,87 +586,87 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I2">
         <v>1970</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M2">
         <v>56985</v>
@@ -691,12 +675,12 @@
         <v>3456789012</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{37ABBD06-7DB8-409A-92FF-467CC21FA30A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{267FAB3B-6E60-4982-8694-49FE14596D68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>